<commit_message>
Add Lucid Trading as 13th firm - complete integration with scoring and UI
</commit_message>
<xml_diff>
--- a/data/futures_prop_firm_database.xlsx
+++ b/data/futures_prop_firm_database.xlsx
@@ -533,7 +533,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1758,6 +1758,94 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Lucid Trading</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>$25K-$150K</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$60-$221 one-time (often 40-50% off)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>6% ($1.5K-$6K)</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>$1.2K-$2.7K (soft breach, none on 25K)</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>$1K-$4.5K EOD trailing</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Trailing (EOD)</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>90/10</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Daily (5 profitable days per cycle)</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>1 day to pass</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Unlimited</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>40% (eval), none on LucidFlex funded</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Rithmic, Tradovate, NinjaTrader, Quantower</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="P14" t="n">
+        <v>2025</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>~15 min payouts, one-time fee, no activation fee, LucidFlex no DLL/consistency</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2663,7 +2751,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3297,6 +3385,53 @@
       <c r="I15" s="13" t="inlineStr">
         <is>
           <t>Varies</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Lucid Trading</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1-step</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>EOD trailing</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Yes (swing trading allowed)</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Yes (up to 5 funded accounts)</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>LucidScale DLL after consistency</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>2-10 minis depending on account</t>
         </is>
       </c>
     </row>
@@ -4050,7 +4185,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4486,6 +4621,38 @@
       <c r="F15" s="15" t="inlineStr">
         <is>
           <t>Instant funding angle</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Lucid Trading</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$30-80</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>40-50% off (SOPF, DGT)</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Monthly</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Fast-growing, strong Discord community</t>
         </is>
       </c>
     </row>

</xml_diff>